<commit_message>
update typo of data
</commit_message>
<xml_diff>
--- a/naics/data/filtered_tic_naics_updated.xlsx
+++ b/naics/data/filtered_tic_naics_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3472D31E-0A7E-264E-9617-0D2BAD9E3657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80CCF5A-12E9-DE4F-BFD0-FFC3947EAADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="847">
   <si>
     <t>tic</t>
   </si>
@@ -2540,9 +2540,6 @@
   </si>
   <si>
     <t>CHK</t>
-  </si>
-  <si>
-    <t> 211120</t>
   </si>
   <si>
     <t>DWAC</t>
@@ -2945,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B846"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A813" zoomScale="66" workbookViewId="0">
+      <selection activeCell="Q837" sqref="Q837"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9659,13 +9656,13 @@
       <c r="A839" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="B839" s="2" t="s">
-        <v>840</v>
+      <c r="B839" s="2">
+        <v>211120</v>
       </c>
     </row>
     <row r="840" spans="1:2">
       <c r="A840" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B840" s="2">
         <v>551112</v>
@@ -9673,7 +9670,7 @@
     </row>
     <row r="841" spans="1:2">
       <c r="A841" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B841" s="2">
         <v>54133</v>
@@ -9681,7 +9678,7 @@
     </row>
     <row r="842" spans="1:2">
       <c r="A842" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B842" s="2">
         <v>458110</v>
@@ -9689,7 +9686,7 @@
     </row>
     <row r="843" spans="1:2">
       <c r="A843" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B843" s="2">
         <v>423490</v>
@@ -9697,7 +9694,7 @@
     </row>
     <row r="844" spans="1:2">
       <c r="A844" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B844" s="2">
         <v>481111</v>
@@ -9705,7 +9702,7 @@
     </row>
     <row r="845" spans="1:2">
       <c r="A845" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B845" s="2">
         <v>522110</v>
@@ -9713,7 +9710,7 @@
     </row>
     <row r="846" spans="1:2">
       <c r="A846" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B846" s="2">
         <v>541870</v>

</xml_diff>